<commit_message>
checkpoint before claude code
</commit_message>
<xml_diff>
--- a/test_results/pipeline_output/statements_shp-afs-2024.xlsx
+++ b/test_results/pipeline_output/statements_shp-afs-2024.xlsx
@@ -527,7 +527,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2026-02-24 11:31:52</t>
+          <t>2026-02-26 18:18:27</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>b2489a4c-8296-454f-b023-fd0916f573fe</t>
+          <t>bee2e2ea-8ce1-49f9-988b-ea69274f6e91</t>
         </is>
       </c>
     </row>

</xml_diff>